<commit_message>
update a few more talks meta data
</commit_message>
<xml_diff>
--- a/_site/assets/datasets/talk-data.xlsx
+++ b/_site/assets/datasets/talk-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="101">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">doi</t>
   </si>
   <si>
+    <t xml:space="preserve">recording</t>
+  </si>
+  <si>
     <t xml:space="preserve">Applying statistical thinking to palaeo data through generalized additive models</t>
   </si>
   <si>
@@ -79,18 +82,81 @@
     <t xml:space="preserve">School of Earth, Environment and Ecosystem Sciences Seminar Series, The Open University, 1st November</t>
   </si>
   <si>
+    <t xml:space="preserve">https://gavinsimpson.github.io/open-university-seminar-nov-2022/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/gavinsimpson/open-university-seminar-nov-2022</t>
+  </si>
+  <si>
     <t xml:space="preserve">Estimating trends in messy time series using generalized additive models</t>
   </si>
   <si>
     <t xml:space="preserve">Statistics &amp; Biostatistic Seminar Series, Department of Statistics &amp; Actuarial Science, University of Waterloo, 10th March</t>
   </si>
   <si>
+    <t xml:space="preserve">https://gavinsimpson.github.io/waterloo2022/slides/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/gavinsimpson/waterloo2022</t>
+  </si>
+  <si>
     <t xml:space="preserve">Quantifying trends in biodiversity with generalized additive models</t>
   </si>
   <si>
     <t xml:space="preserve">National Centre for Statistical Ecology seminar series, 9th February</t>
   </si>
   <si>
+    <t xml:space="preserve">https://gavinsimpson.github.io/ncse-seminar-2022/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/gavinsimpson/ncse-seminar-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.5281/zenodo.6033545</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detecting change in palaeoecological time series, old and new</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PaleoEcoGen seminar series, online, 24</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> March</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://gavinsimpson.github.io/paleoecogen-seminar-2022/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/gavinsimpson/paleoecogen-seminar-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/4qN5l6zI0nk</t>
+  </si>
+  <si>
     <t xml:space="preserve">Generalized Additive Models with R and mgcv</t>
   </si>
   <si>
@@ -214,10 +280,25 @@
     <t xml:space="preserve">Joint Ecological Society of America and Canadian Society of Ecology and Evolution Annual Meeting, Montreal, 14-19 August, 2022</t>
   </si>
   <si>
+    <t xml:space="preserve">https://gavinsimpson.github.io/esa-csee-2022/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/gavinsimpson/esa-csee-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.5281/zenodo.7003948</t>
+  </si>
+  <si>
     <t xml:space="preserve">Estimating the time-varying correlation between time series using copula distributional models</t>
   </si>
   <si>
     <t xml:space="preserve">Virtual International Statistical Ecology Conference (vISEC) 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://gavinsimpson.github.io/visec2020-talk/visec2020-simpson-june-2020.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/gavinsimpson/visec2020-talk</t>
   </si>
   <si>
     <t xml:space="preserve">Estimating continuous measures of ecological resilience from palaeoecological time series</t>
@@ -280,7 +361,7 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -301,6 +382,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -375,13 +463,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.69"/>
@@ -412,16 +500,19 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>45126</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -432,13 +523,13 @@
         <v>1</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -446,10 +537,10 @@
         <v>44993</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -460,10 +551,10 @@
         <v>0</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,10 +562,10 @@
         <v>44866</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -483,17 +574,23 @@
       <c r="E4" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>44632</v>
+        <v>44630</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -502,6 +599,12 @@
       <c r="E5" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -509,10 +612,10 @@
         <v>44601</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -522,35 +625,51 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>44564</v>
+        <v>44644</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>44517</v>
+        <v>44564</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -563,13 +682,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>44498</v>
+        <v>44517</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -582,13 +701,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>44477</v>
+        <v>44498</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -601,13 +720,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>44400</v>
+        <v>44477</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D11" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -620,13 +739,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>43983</v>
+        <v>44400</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D12" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -642,10 +761,10 @@
         <v>43983</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D13" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -658,13 +777,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>43647</v>
+        <v>43983</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D14" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -677,13 +796,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>43405</v>
+        <v>43647</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="D15" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -696,13 +815,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>43344</v>
+        <v>43405</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D16" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -715,13 +834,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>43009</v>
+        <v>43344</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D17" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -734,13 +853,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>42736</v>
+        <v>43009</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D18" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -753,13 +872,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>42217</v>
+        <v>42736</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="D19" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -772,13 +891,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>40878</v>
+        <v>42217</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D20" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -791,13 +910,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>40118</v>
+        <v>40878</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D21" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -810,13 +929,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>39142</v>
+        <v>40118</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D22" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -829,13 +948,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>38473</v>
+        <v>39142</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D23" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -848,13 +967,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>38108</v>
+        <v>38473</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D24" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -867,41 +986,32 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>45083</v>
+        <v>38108</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D25" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="E25" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>44774</v>
+        <v>45083</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D26" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -910,17 +1020,26 @@
       <c r="E26" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>43983</v>
+        <v>44774</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="D27" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -929,17 +1048,26 @@
       <c r="E27" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>43647</v>
+        <v>43983</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="D28" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -948,17 +1076,23 @@
       <c r="E28" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
-        <v>43586</v>
+        <v>43647</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D29" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -971,13 +1105,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
-        <v>43313</v>
+        <v>43586</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="D30" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -990,13 +1124,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
-        <v>43282</v>
+        <v>43313</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="D31" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1009,13 +1143,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
-        <v>43252</v>
+        <v>43282</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="D32" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1028,13 +1162,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
-        <v>42948</v>
+        <v>43252</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="D33" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1047,13 +1181,13 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
-        <v>42583</v>
+        <v>42948</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="D34" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1066,13 +1200,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
-        <v>42552</v>
+        <v>42583</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="D35" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1085,19 +1219,38 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
+        <v>42552</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="n">
         <v>42005</v>
       </c>
-      <c r="B36" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="2" t="n">
+      <c r="B37" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>